<commit_message>
Site updated: 2021-10-05 14:12:59
</commit_message>
<xml_diff>
--- a/draft/模型性能评估_V1_1.xlsx
+++ b/draft/模型性能评估_V1_1.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WorkSpace\GitHub\HexoBlog\source\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4028794F-20ED-4338-A9A4-9628775F3060}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500DB212-CCA4-4FE6-A9FF-91D8761D287C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -186,14 +186,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>编译出错</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ncsdk nnpu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>可编译，运行时出错</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -202,10 +194,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>编译出错，维度不匹配</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>model-01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -222,11 +210,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>batch_normal错误</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>运行时错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model-01-half-right</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>conv_transpose(group &gt; 1)</t>
+  </si>
+  <si>
+    <t>conv_transpose(group &gt; 1)
+目前不支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model-small</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>\</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>推理时延(ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>训练值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> nnpu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PowerVR ncsdk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TVM 08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吞吐量(fps)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实际</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model-01-half-left</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,7 +441,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -442,6 +478,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -489,7 +537,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -775,61 +844,61 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:E14"/>
+      <selection activeCell="G3" sqref="G3:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.5" style="12" customWidth="1"/>
-    <col min="2" max="2" width="16.375" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
     <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="14.75" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="11.375" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-    </row>
-    <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="18" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="21"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
@@ -843,14 +912,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="28" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2">
@@ -865,14 +934,14 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="25"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="2">
         <v>2440</v>
       </c>
@@ -885,14 +954,14 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="25"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="2">
         <v>620</v>
       </c>
@@ -901,14 +970,14 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="25"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
@@ -919,14 +988,14 @@
         <v>3.23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="25"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="2">
         <v>164</v>
       </c>
@@ -935,14 +1004,14 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="25"/>
+      <c r="C9" s="29"/>
       <c r="D9" s="2">
         <v>316</v>
       </c>
@@ -959,14 +1028,14 @@
         <v>573</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="25"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="2">
         <v>50.5</v>
       </c>
@@ -983,26 +1052,26 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="22" t="s">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="25"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
       <c r="B12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="25"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1019,14 +1088,14 @@
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="25"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="2">
         <v>41</v>
       </c>
@@ -1037,14 +1106,14 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1055,17 +1124,17 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1095,14 +1164,14 @@
       <selection activeCell="C3" sqref="C3:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.75" customWidth="1"/>
     <col min="2" max="2" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1115,8 +1184,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="31"/>
       <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
@@ -1127,8 +1196,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="4">
@@ -1139,8 +1208,8 @@
       </c>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="29"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="33"/>
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -1151,8 +1220,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="33"/>
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -1163,8 +1232,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="33"/>
       <c r="B6" s="4">
         <v>4</v>
       </c>
@@ -1173,8 +1242,8 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="29"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="33"/>
       <c r="B7" s="4">
         <v>5</v>
       </c>
@@ -1183,8 +1252,8 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="30"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="34"/>
       <c r="B8" s="4">
         <v>6</v>
       </c>
@@ -1208,143 +1277,286 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F992FC-063B-4545-A80C-C4AEDBDC4F1F}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9" style="3"/>
-    <col min="3" max="3" width="24.875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="17" style="3" customWidth="1"/>
+    <col min="2" max="2" width="7.08203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23" style="3" customWidth="1"/>
+    <col min="5" max="6" width="9.25" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="31"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="13" t="s">
+      <c r="C1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="E2" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="41"/>
+      <c r="G3" s="38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="37"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="39"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="D5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="40"/>
       <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="33"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="13">
         <v>7.74</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="C9" s="6">
+        <v>15</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B10" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="14">
+      <c r="D10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1300</v>
+      </c>
+      <c r="D11" s="14">
         <v>994</v>
       </c>
-      <c r="D7" s="14">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="E11" s="16">
+        <v>294</v>
+      </c>
+      <c r="F11" s="16">
+        <v>340</v>
+      </c>
+      <c r="G11" s="16">
+        <f t="shared" ref="G11:G14" si="0">1000/F11</f>
+        <v>2.9411764705882355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="3">
+        <v>99</v>
+      </c>
+      <c r="F12" s="3">
+        <v>126</v>
+      </c>
+      <c r="G12" s="16">
+        <f t="shared" si="0"/>
+        <v>7.9365079365079367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="14">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D8" s="14">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="14" t="s">
+      <c r="B13" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="16">
+        <v>138</v>
+      </c>
+      <c r="F13" s="16">
+        <v>241</v>
+      </c>
+      <c r="G13" s="16">
+        <f t="shared" si="0"/>
+        <v>4.1493775933609962</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
         <v>47</v>
       </c>
+      <c r="B14" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="15">
+        <v>716</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="16">
+        <v>183</v>
+      </c>
+      <c r="F14" s="16">
+        <v>205</v>
+      </c>
+      <c r="G14" s="16">
+        <f t="shared" si="0"/>
+        <v>4.8780487804878048</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:D1"/>
+  <mergeCells count="10">
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D2:D4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>